<commit_message>
added PZN and PZS to trt
</commit_message>
<xml_diff>
--- a/AWQP Water Processing ID Key_2023.xlsx
+++ b/AWQP Water Processing ID Key_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ-CPU\Documents\GitHub\ALS-Data-Cleaning-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9D2298-4E75-4439-860A-D2C11A2C0821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB98FBE-0DBE-4073-8F91-21E6E66ABF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="5400" windowWidth="14400" windowHeight="15750" xr2:uid="{80777274-BFA3-44C9-A50F-B90CEE9B5D11}"/>
+    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15990" xr2:uid="{80777274-BFA3-44C9-A50F-B90CEE9B5D11}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="214">
   <si>
     <t>Location</t>
   </si>
@@ -1350,6 +1350,18 @@
   </si>
   <si>
     <t>The sheet titled, "Example Event List 2023" contains a list of example ID's made for sample bottle preparation for lab submittal and documentation</t>
+  </si>
+  <si>
+    <t>PZN</t>
+  </si>
+  <si>
+    <t>PZS</t>
+  </si>
+  <si>
+    <t>Piezometer North</t>
+  </si>
+  <si>
+    <t>Piezometer South</t>
   </si>
 </sst>
 </file>
@@ -1848,6 +1860,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1857,8 +1871,6 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1888,10 +1900,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2200,7 +2208,7 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="41" t="s">
         <v>205</v>
       </c>
     </row>
@@ -2225,7 +2233,7 @@
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="40" t="s">
         <v>204</v>
       </c>
     </row>
@@ -2260,7 +2268,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2557,10 +2565,10 @@
         <v>48</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>79</v>
+        <v>212</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>66</v>
+        <v>210</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="29" t="s">
@@ -2580,10 +2588,10 @@
         <v>50</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>80</v>
+        <v>213</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>67</v>
+        <v>211</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="29" t="s">
@@ -2603,10 +2611,10 @@
         <v>52</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G16" s="30" t="s">
         <v>111</v>
@@ -2625,10 +2633,10 @@
         <v>53</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G17" s="29" t="s">
         <v>112</v>
@@ -2642,10 +2650,10 @@
         <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -2656,10 +2664,10 @@
         <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>87</v>
@@ -2676,10 +2684,10 @@
         <v>123</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>4</v>
@@ -2695,6 +2703,12 @@
       <c r="B21" s="5" t="s">
         <v>89</v>
       </c>
+      <c r="D21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G21" s="1" t="s">
         <v>12</v>
       </c>
@@ -2708,6 +2722,12 @@
       </c>
       <c r="B22" s="1" t="s">
         <v>196</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -2832,10 +2852,10 @@
       <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="41"/>
+      <c r="B35" s="43"/>
       <c r="D35" s="33" t="s">
         <v>102</v>
       </c>
@@ -2948,7 +2968,7 @@
       </c>
       <c r="C2" s="38">
         <f t="shared" ref="C2:C49" ca="1" si="0">TODAY()</f>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>136</v>
@@ -2973,7 +2993,7 @@
       </c>
       <c r="C3" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -2988,16 +3008,16 @@
       <c r="G3" s="1">
         <v>125</v>
       </c>
-      <c r="K3" s="42" t="s">
+      <c r="K3" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
@@ -3008,7 +3028,7 @@
       </c>
       <c r="C4" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -3023,14 +3043,14 @@
       <c r="G4" s="1">
         <v>125</v>
       </c>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="42"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
@@ -3041,7 +3061,7 @@
       </c>
       <c r="C5" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
@@ -3056,14 +3076,14 @@
       <c r="G5" s="1">
         <v>125</v>
       </c>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
@@ -3074,7 +3094,7 @@
       </c>
       <c r="C6" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>146</v>
@@ -3089,14 +3109,14 @@
       <c r="G6" s="1">
         <v>125</v>
       </c>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
@@ -3107,7 +3127,7 @@
       </c>
       <c r="C7" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>149</v>
@@ -3122,14 +3142,14 @@
       <c r="G7" s="1">
         <v>125</v>
       </c>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="42"/>
-      <c r="P7" s="42"/>
-      <c r="Q7" s="42"/>
-      <c r="R7" s="42"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="44"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
@@ -3140,7 +3160,7 @@
       </c>
       <c r="C8" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>136</v>
@@ -3155,14 +3175,14 @@
       <c r="G8" s="1">
         <v>125</v>
       </c>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="42"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
@@ -3173,7 +3193,7 @@
       </c>
       <c r="C9" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -3188,14 +3208,14 @@
       <c r="G9" s="1">
         <v>125</v>
       </c>
-      <c r="K9" s="42"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="42"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="42"/>
-      <c r="R9" s="42"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="44"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
@@ -3206,7 +3226,7 @@
       </c>
       <c r="C10" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>6</v>
@@ -3221,14 +3241,14 @@
       <c r="G10" s="1">
         <v>125</v>
       </c>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="42"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="44"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
@@ -3239,7 +3259,7 @@
       </c>
       <c r="C11" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>18</v>
@@ -3264,7 +3284,7 @@
       </c>
       <c r="C12" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>146</v>
@@ -3289,7 +3309,7 @@
       </c>
       <c r="C13" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>149</v>
@@ -3317,7 +3337,7 @@
       </c>
       <c r="C14" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>136</v>
@@ -3345,7 +3365,7 @@
       </c>
       <c r="C15" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -3374,7 +3394,7 @@
       </c>
       <c r="C16" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
@@ -3403,7 +3423,7 @@
       </c>
       <c r="C17" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>18</v>
@@ -3428,7 +3448,7 @@
       </c>
       <c r="C18" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>146</v>
@@ -3453,7 +3473,7 @@
       </c>
       <c r="C19" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>149</v>
@@ -3478,7 +3498,7 @@
       </c>
       <c r="C20" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>136</v>
@@ -3503,7 +3523,7 @@
       </c>
       <c r="C21" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>11</v>
@@ -3528,7 +3548,7 @@
       </c>
       <c r="C22" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>6</v>
@@ -3553,7 +3573,7 @@
       </c>
       <c r="C23" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>18</v>
@@ -3578,7 +3598,7 @@
       </c>
       <c r="C24" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>146</v>
@@ -3603,7 +3623,7 @@
       </c>
       <c r="C25" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>149</v>
@@ -3628,7 +3648,7 @@
       </c>
       <c r="C26" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>136</v>
@@ -3653,7 +3673,7 @@
       </c>
       <c r="C27" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>11</v>
@@ -3678,7 +3698,7 @@
       </c>
       <c r="C28" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>6</v>
@@ -3703,7 +3723,7 @@
       </c>
       <c r="C29" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>18</v>
@@ -3728,7 +3748,7 @@
       </c>
       <c r="C30" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>146</v>
@@ -3753,7 +3773,7 @@
       </c>
       <c r="C31" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>149</v>
@@ -3778,7 +3798,7 @@
       </c>
       <c r="C32" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>136</v>
@@ -3803,7 +3823,7 @@
       </c>
       <c r="C33" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>11</v>
@@ -3828,7 +3848,7 @@
       </c>
       <c r="C34" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>6</v>
@@ -3853,7 +3873,7 @@
       </c>
       <c r="C35" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>18</v>
@@ -3878,7 +3898,7 @@
       </c>
       <c r="C36" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>146</v>
@@ -3903,7 +3923,7 @@
       </c>
       <c r="C37" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>149</v>
@@ -3928,7 +3948,7 @@
       </c>
       <c r="C38" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>136</v>
@@ -3953,7 +3973,7 @@
       </c>
       <c r="C39" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -3978,7 +3998,7 @@
       </c>
       <c r="C40" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>6</v>
@@ -4003,7 +4023,7 @@
       </c>
       <c r="C41" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>18</v>
@@ -4028,7 +4048,7 @@
       </c>
       <c r="C42" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>146</v>
@@ -4053,7 +4073,7 @@
       </c>
       <c r="C43" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>149</v>
@@ -4078,7 +4098,7 @@
       </c>
       <c r="C44" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>136</v>
@@ -4103,7 +4123,7 @@
       </c>
       <c r="C45" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
@@ -4128,7 +4148,7 @@
       </c>
       <c r="C46" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>6</v>
@@ -4153,7 +4173,7 @@
       </c>
       <c r="C47" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>18</v>
@@ -4178,7 +4198,7 @@
       </c>
       <c r="C48" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>146</v>
@@ -4203,7 +4223,7 @@
       </c>
       <c r="C49" s="38">
         <f t="shared" ca="1" si="0"/>
-        <v>45168</v>
+        <v>45245</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>149</v>
@@ -6497,6 +6517,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="167cb1e9-24b5-43e0-9f5d-14a54474cc90">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fbf6f0f6-9634-473c-8838-2f74fc79f714" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100678F2DA36292A241BB6B602A04ACAAD9" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8d9fb0f190deb5e7e937e6d8ad317d77">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="167cb1e9-24b5-43e0-9f5d-14a54474cc90" xmlns:ns3="fbf6f0f6-9634-473c-8838-2f74fc79f714" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="211896cd03a7fb44aac70cae515804dc" ns2:_="" ns3:_="">
     <xsd:import namespace="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
@@ -6745,27 +6785,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="167cb1e9-24b5-43e0-9f5d-14a54474cc90">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fbf6f0f6-9634-473c-8838-2f74fc79f714" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A9A0347-3472-4A1D-8404-53EC21279416}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6928EB07-F497-4032-8701-AD7E4A30F74A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
+    <ds:schemaRef ds:uri="fbf6f0f6-9634-473c-8838-2f74fc79f714"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9D94A9-9B75-47D0-9DB5-A09B822864E6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6782,23 +6821,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6928EB07-F497-4032-8701-AD7E4A30F74A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
-    <ds:schemaRef ds:uri="fbf6f0f6-9634-473c-8838-2f74fc79f714"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A9A0347-3472-4A1D-8404-53EC21279416}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>